<commit_message>
Excellent version of the lab! Few data feeds for outputs of rolling processes, such as concrete reba, that produce more than one product, still produce misaligned ALANG commands (coefficient added that is smaller than 1). Needs to be fixed.
</commit_message>
<xml_diff>
--- a/Settings/Base/IE_settings.xlsx
+++ b/Settings/Base/IE_settings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="factors" sheetId="1" r:id="rId1"/>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -588,7 +588,7 @@
         <v>16</v>
       </c>
       <c r="B2">
-        <v>20200426</v>
+        <v>20200428</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -604,7 +604,7 @@
         <v>30</v>
       </c>
       <c r="B4">
-        <v>20200426</v>
+        <v>20200428</v>
       </c>
     </row>
   </sheetData>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -642,10 +642,10 @@
         <v>20</v>
       </c>
       <c r="B2">
+        <v>0.2</v>
+      </c>
+      <c r="C2">
         <v>1</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -653,13 +653,13 @@
         <v>21</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -678,10 +678,10 @@
         <v>23</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -689,10 +689,10 @@
         <v>24</v>
       </c>
       <c r="B6">
+        <v>0.2</v>
+      </c>
+      <c r="C6">
         <v>1</v>
-      </c>
-      <c r="C6">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -722,7 +722,7 @@
         <v>27</v>
       </c>
       <c r="D9">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version works fine. Still unrealistic numbers in SUTs which may be due to the incorrect implementation of the WIO module.
</commit_message>
<xml_diff>
--- a/Settings/Base/IE_settings.xlsx
+++ b/Settings/Base/IE_settings.xlsx
@@ -110,10 +110,10 @@
     <t>WSA</t>
   </si>
   <si>
-    <t>V4</t>
-  </si>
-  <si>
     <t>Additional</t>
+  </si>
+  <si>
+    <t>V5</t>
   </si>
 </sst>
 </file>
@@ -567,7 +567,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -596,15 +596,15 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4">
-        <v>20200428</v>
+        <v>20200429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Still, WSA feed not function correctly. AISHA is probably misinterpreting the commands.
</commit_message>
<xml_diff>
--- a/Settings/Base/IE_settings.xlsx
+++ b/Settings/Base/IE_settings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="factors" sheetId="1" r:id="rId1"/>
@@ -566,7 +566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -642,10 +642,10 @@
         <v>20</v>
       </c>
       <c r="B2">
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -653,13 +653,13 @@
         <v>21</v>
       </c>
       <c r="B3">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Ratio constraints implemented and tested.
</commit_message>
<xml_diff>
--- a/Settings/Base/IE_settings.xlsx
+++ b/Settings/Base/IE_settings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="factors" sheetId="1" r:id="rId1"/>
@@ -443,8 +443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -465,7 +465,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>2.2999999999999998</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -473,7 +473,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -481,7 +481,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>1.35</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -489,7 +489,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="2">
-        <v>0.36</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -497,7 +497,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -505,7 +505,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -647,6 +647,9 @@
       <c r="C2">
         <v>10</v>
       </c>
+      <c r="D2">
+        <v>1000000</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -659,7 +662,7 @@
         <v>10</v>
       </c>
       <c r="D3">
-        <v>1000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -720,9 +723,6 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
-      </c>
-      <c r="D9">
-        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New version of data feeds work but problem with the industry balance.
</commit_message>
<xml_diff>
--- a/Settings/Base/IE_settings.xlsx
+++ b/Settings/Base/IE_settings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="factors" sheetId="1" r:id="rId1"/>
@@ -443,7 +443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +642,7 @@
         <v>20</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -656,7 +656,7 @@
         <v>21</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -670,7 +670,7 @@
         <v>22</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -681,10 +681,10 @@
         <v>23</v>
       </c>
       <c r="B5">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -692,10 +692,10 @@
         <v>24</v>
       </c>
       <c r="B6">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -703,7 +703,7 @@
         <v>25</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -714,7 +714,7 @@
         <v>26</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>10</v>

</xml_diff>